<commit_message>
Adjust tests for new restrictions
</commit_message>
<xml_diff>
--- a/tests/integration/test_files/foreign_key_violated.xlsx
+++ b/tests/integration/test_files/foreign_key_violated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmartinez/repos/set-aside/pdcm-lectern-validator/tests/integration/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7C0E2B-EEAB-5940-BA5B-C8CDCB718682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61557059-BDFA-0C43-9636-9A0D448E8955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10420" yWindow="6180" windowWidth="29040" windowHeight="11680" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9360" yWindow="6180" windowWidth="29040" windowHeight="11680" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="122">
   <si>
     <t>patient_id</t>
   </si>
@@ -378,9 +378,6 @@
     <t>https://tumor.informatics.jax.org</t>
   </si>
   <si>
-    <t>CRC001asdas4LM</t>
-  </si>
-  <si>
     <t>industry</t>
   </si>
   <si>
@@ -460,9 +457,6 @@
   </si>
   <si>
     <t>not provided</t>
-  </si>
-  <si>
-    <t>CRC0014LM_2</t>
   </si>
   <si>
     <t>A0088_X</t>
@@ -1242,14 +1236,14 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>85</v>
@@ -1258,7 +1252,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1"/>
@@ -1531,24 +1525,24 @@
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>36</v>
@@ -1566,7 +1560,7 @@
       </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>42</v>
@@ -1574,7 +1568,7 @@
       <c r="R3" s="4"/>
       <c r="S3" s="15"/>
       <c r="T3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" customHeight="1"/>
@@ -2639,31 +2633,31 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>56</v>
       </c>
       <c r="G3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1"/>
@@ -3700,16 +3694,16 @@
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>54</v>
@@ -3726,7 +3720,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3764,8 +3758,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="102">
-      <c r="A2" s="24" t="s">
-        <v>52</v>
+      <c r="A2" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>83</v>
@@ -3774,7 +3768,7 @@
         <v>89</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="26" t="s">
         <v>52</v>
@@ -3783,10 +3777,10 @@
         <v>84</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H2" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>58</v>
@@ -3796,28 +3790,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="102">
-      <c r="A3" s="24" t="s">
-        <v>122</v>
+      <c r="A3" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>83</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H3" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J3" s="24" t="s">
         <v>59</v>
@@ -3844,8 +3838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMI4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -3889,7 +3883,7 @@
     </row>
     <row r="2" spans="1:1023" ht="34">
       <c r="A2" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>91</v>
@@ -3912,14 +3906,14 @@
     </row>
     <row r="3" spans="1:1023" ht="170.75" customHeight="1">
       <c r="A3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>74</v>

</xml_diff>